<commit_message>
updated code up to unify base files
</commit_message>
<xml_diff>
--- a/data/_metadata/dicts/raw_SIMAT_2017-2023.xlsx
+++ b/data/_metadata/dicts/raw_SIMAT_2017-2023.xlsx
@@ -1,420 +1,413 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajoseguerrero/Documents/Secretaria de Educación/Deserción Escolar/school_dropout/data/metadata/dicts/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EF2932-977F-8C48-B95B-0D3CB8C15701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="colname" sheetId="1" r:id="rId1"/>
-    <sheet name="colclass" sheetId="2" r:id="rId2"/>
+    <sheet name="colname" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="colclass" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="129">
-  <si>
-    <t>uniname</t>
-  </si>
-  <si>
-    <t>uniclass</t>
-  </si>
-  <si>
-    <t>class_mode</t>
-  </si>
-  <si>
-    <t>unique_classes</t>
-  </si>
-  <si>
-    <t>coverage</t>
-  </si>
-  <si>
-    <t>MEDELLIN_2017.parquet</t>
-  </si>
-  <si>
-    <t>MEDELLIN_2018.parquet</t>
-  </si>
-  <si>
-    <t>MEDELLIN_2019.parquet</t>
-  </si>
-  <si>
-    <t>MEDELLIN_2020.parquet</t>
-  </si>
-  <si>
-    <t>MEDELLIN_2021.parquet</t>
-  </si>
-  <si>
-    <t>MEDELLIN_2022.parquet</t>
-  </si>
-  <si>
-    <t>MEDELLIN_2023.parquet</t>
-  </si>
-  <si>
-    <t>ANNO_INF</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>integer; numeric</t>
-  </si>
-  <si>
-    <t>APELLIDO1</t>
-  </si>
-  <si>
-    <t>character</t>
-  </si>
-  <si>
-    <t>APELLIDO2</t>
-  </si>
-  <si>
-    <t>BEN_HER_NAC</t>
-  </si>
-  <si>
-    <t>BEN_MAD_FLIA</t>
-  </si>
-  <si>
-    <t>BEN_VET_FP</t>
-  </si>
-  <si>
-    <t>CAB_FAMILIA</t>
-  </si>
-  <si>
-    <t>CARACTER</t>
-  </si>
-  <si>
-    <t>CODIGO_DANE</t>
-  </si>
-  <si>
-    <t>integer64</t>
-  </si>
-  <si>
-    <t>integer64; character; numeric</t>
-  </si>
-  <si>
-    <t>CODIGO_DANE_SEDE</t>
-  </si>
-  <si>
-    <t>CODIGO_SED</t>
-  </si>
-  <si>
-    <t>CON_ALUM_ANO_ANT</t>
-  </si>
-  <si>
-    <t>integer; logical</t>
-  </si>
-  <si>
-    <t>CONS_SEDE</t>
-  </si>
-  <si>
-    <t>integer64; character</t>
-  </si>
-  <si>
-    <t>CTE_ID_APOYO_ACAD_ESP</t>
-  </si>
-  <si>
-    <t>character; numeric</t>
-  </si>
-  <si>
-    <t>CTE_ID_CALENDARIO</t>
-  </si>
-  <si>
-    <t>integer; character; numeric</t>
-  </si>
-  <si>
-    <t>CTE_ID_SECTOR</t>
-  </si>
-  <si>
-    <t>CTE_ID_SRPA</t>
-  </si>
-  <si>
-    <t>CTE_ID_ZONA</t>
-  </si>
-  <si>
-    <t>DIRECCION_RESIDENCIA</t>
-  </si>
-  <si>
-    <t>DISCAPACIDAD1</t>
-  </si>
-  <si>
-    <t>DIVIPOLA_MUNICIPIO</t>
-  </si>
-  <si>
-    <t>Divipola_MUNICIPIO</t>
-  </si>
-  <si>
-    <t>DPTO_CARGA</t>
-  </si>
-  <si>
-    <t>EDAD</t>
-  </si>
-  <si>
-    <t>EFICIENCIA</t>
-  </si>
-  <si>
-    <t>ESPECIALIDAD</t>
-  </si>
-  <si>
-    <t>EST_ID</t>
-  </si>
-  <si>
-    <t>ESTADO</t>
-  </si>
-  <si>
-    <t>ESTRATO</t>
-  </si>
-  <si>
-    <t>ETNIA</t>
-  </si>
-  <si>
-    <t>FECHA_NACIMIENTO</t>
-  </si>
-  <si>
-    <t>character; POSIXct;POSIXt</t>
-  </si>
-  <si>
-    <t>FECHA_NOVEDAD</t>
-  </si>
-  <si>
-    <t>FUE_RECU</t>
-  </si>
-  <si>
-    <t>GENERO</t>
-  </si>
-  <si>
-    <t>GRADO</t>
-  </si>
-  <si>
-    <t>GRADO1</t>
-  </si>
-  <si>
-    <t>grado1</t>
-  </si>
-  <si>
-    <t>GRUPO</t>
-  </si>
-  <si>
-    <t>METODOLOGIA</t>
-  </si>
-  <si>
-    <t>MUN_CODIGO</t>
-  </si>
-  <si>
-    <t>NAC_DEPTO</t>
-  </si>
-  <si>
-    <t>NAC_MUN</t>
-  </si>
-  <si>
-    <t>NIVEL5</t>
-  </si>
-  <si>
-    <t>NOMBRE_ESTABLECIMIENTO</t>
-  </si>
-  <si>
-    <t>NOMBRE_SEDE</t>
-  </si>
-  <si>
-    <t>NOMBRE1</t>
-  </si>
-  <si>
-    <t>NOMBRE2</t>
-  </si>
-  <si>
-    <t>NRO_DOCUMENTO</t>
-  </si>
-  <si>
-    <t>NUEVO</t>
-  </si>
-  <si>
-    <t>PER_ID</t>
-  </si>
-  <si>
-    <t>PROVIENE_OTRO_MUN</t>
-  </si>
-  <si>
-    <t>character; logical</t>
-  </si>
-  <si>
-    <t>PROVIENE_SECTOR_PRIV</t>
-  </si>
-  <si>
-    <t>REPITENCIA_FINAL</t>
-  </si>
-  <si>
-    <t>integer; character</t>
-  </si>
-  <si>
-    <t>Repitencia_Final</t>
-  </si>
-  <si>
-    <t>REPITENTE</t>
-  </si>
-  <si>
-    <t>RES</t>
-  </si>
-  <si>
-    <t>RES_DEPTO</t>
-  </si>
-  <si>
-    <t>RES_MUN</t>
-  </si>
-  <si>
-    <t>SECTOR_MATR</t>
-  </si>
-  <si>
-    <t>SEDE_ID</t>
-  </si>
-  <si>
-    <t>SISBEN</t>
-  </si>
-  <si>
-    <t>SIT_ACAD_ANO_ANT</t>
-  </si>
-  <si>
-    <t>SUBSIDIADO</t>
-  </si>
-  <si>
-    <t>TEL</t>
-  </si>
-  <si>
-    <t>TIPO_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>TIPO_DOCUMENTO</t>
-  </si>
-  <si>
-    <t>TIPO_JORNADA</t>
-  </si>
-  <si>
-    <t>TOTAL_MATRICULA</t>
-  </si>
-  <si>
-    <t>ZON_ALU</t>
-  </si>
-  <si>
-    <t>CAP_EXC</t>
-  </si>
-  <si>
-    <t>CODIGO_PAIS_ORIGEN</t>
-  </si>
-  <si>
-    <t>ETNIA1</t>
-  </si>
-  <si>
-    <t>INS_FAMILIAR</t>
-  </si>
-  <si>
-    <t>INTERNADO</t>
-  </si>
-  <si>
-    <t>MATRICULA_DEFINITIVA</t>
-  </si>
-  <si>
-    <t>Matricula_Definitiva</t>
-  </si>
-  <si>
-    <t>MOTIVO_RETIRO</t>
-  </si>
-  <si>
-    <t>NOMBRE_PAIS_ORIGEN</t>
-  </si>
-  <si>
-    <t>TRASTORNOS_ESPECIFICOS</t>
-  </si>
-  <si>
-    <t>DISCAPACIDAD_HOMOLGADA_2021</t>
-  </si>
-  <si>
-    <t>31/03/2024</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>CAP_EXC2</t>
-  </si>
-  <si>
-    <t>COLUMNA1</t>
-  </si>
-  <si>
-    <t>logical</t>
-  </si>
-  <si>
-    <t>Columna1</t>
-  </si>
-  <si>
-    <t>DISCAP_HOMOLGADA_2021</t>
-  </si>
-  <si>
-    <t>DPTO_EXP</t>
-  </si>
-  <si>
-    <t>EDAD DEFNITIVA</t>
-  </si>
-  <si>
-    <t>ESTADO_DEFINITIVO</t>
-  </si>
-  <si>
-    <t>ESTADO_ESTABLEC</t>
-  </si>
-  <si>
-    <t>Estado_Establec</t>
-  </si>
-  <si>
-    <t>ESTADO_SEDE</t>
-  </si>
-  <si>
-    <t>Estado_Sede</t>
-  </si>
-  <si>
-    <t>EXP_DEPTO</t>
-  </si>
-  <si>
-    <t>EXP_MUN</t>
-  </si>
-  <si>
-    <t>INTERNADO_AJ</t>
-  </si>
-  <si>
-    <t>INTERNADO_aj</t>
-  </si>
-  <si>
-    <t>MOTIVO</t>
-  </si>
-  <si>
-    <t>MUN_EXP</t>
-  </si>
-  <si>
-    <t>POB_VICT_CONF</t>
-  </si>
-  <si>
-    <t>SECTOR_CONPES</t>
-  </si>
-  <si>
-    <t>VAL_DES_PERIODO1</t>
-  </si>
-  <si>
-    <t>VAL_DES_PERIODO2</t>
-  </si>
-  <si>
-    <t>POSIXct;POSIXt</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+  <si>
+    <t xml:space="preserve">uniname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uniclass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">class_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique_classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDELLIN_2017.parquet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDELLIN_2018.parquet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDELLIN_2019.parquet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDELLIN_2020.parquet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDELLIN_2021.parquet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDELLIN_2022.parquet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDELLIN_2023.parquet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANNO_INF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer; numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APELLIDO1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APELLIDO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEN_HER_NAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEN_MAD_FLIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEN_VET_FP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAB_FAMILIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARACTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODIGO_DANE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer64; character; numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODIGO_DANE_SEDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODIGO_SED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CON_ALUM_ANO_ANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer; logical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONS_SEDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer64; character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTE_ID_APOYO_ACAD_ESP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character; numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTE_ID_CALENDARIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer; character; numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTE_ID_SECTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTE_ID_SRPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTE_ID_ZONA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIRECCION_RESIDENCIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCAPACIDAD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIVIPOLA_MUNICIPIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divipola_MUNICIPIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPTO_CARGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EFICIENCIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESPECIALIDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EST_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTRATO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETNIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA_NACIMIENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character; POSIXct;POSIXt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA_NOVEDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUE_RECU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRADO1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grado1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRUPO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METODOLOGIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUN_CODIGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAC_DEPTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAC_MUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIVEL5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE_ESTABLECIMIENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE_SEDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRO_DOCUMENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUEVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PER_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROVIENE_OTRO_MUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character; logical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROVIENE_SECTOR_PRIV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPITENCIA_FINAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer; character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repitencia_Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPITENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_DEPTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_MUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTOR_MATR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEDE_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SISBEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIT_ACAD_ANO_ANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBSIDIADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIPO_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIPO_DOCUMENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIPO_JORNADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL_MATRICULA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZON_ALU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP_EXC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODIGO_PAIS_ORIGEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETNIA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INS_FAMILIAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERNADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATRICULA_DEFINITIVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matricula_Definitiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOTIVO_RETIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE_PAIS_ORIGEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRASTORNOS_ESPECIFICOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCAPACIDAD_HOMOLGADA_2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31/03/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP_EXC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMNA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columna1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCAP_HOMOLGADA_2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPTO_EXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD DEFNITIVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTADO_DEFINITIVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTADO_ESTABLEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estado_Establec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTADO_SEDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estado_Sede</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXP_DEPTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXP_MUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERNADO_AJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERNADO_aj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOTIVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUN_EXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POB_VICT_CONF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTOR_CONPES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAL_DES_PERIODO1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAL_DES_PERIODO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSIXct;POSIXt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -450,15 +443,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -740,20 +724,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L95"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -791,17 +769,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
+      <c r="B2"/>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>100</v>
       </c>
       <c r="F2" t="s">
@@ -826,7 +805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -839,7 +818,7 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>100</v>
       </c>
       <c r="F3" t="s">
@@ -864,7 +843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -877,7 +856,7 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>100</v>
       </c>
       <c r="F4" t="s">
@@ -902,7 +881,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -915,7 +894,7 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>100</v>
       </c>
       <c r="F5" t="s">
@@ -940,7 +919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -953,7 +932,7 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>100</v>
       </c>
       <c r="F6" t="s">
@@ -978,7 +957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -991,7 +970,7 @@
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>100</v>
       </c>
       <c r="F7" t="s">
@@ -1016,7 +995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1029,7 +1008,7 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>100</v>
       </c>
       <c r="F8" t="s">
@@ -1054,17 +1033,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>22</v>
       </c>
+      <c r="B9"/>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>100</v>
       </c>
       <c r="F9" t="s">
@@ -1089,17 +1069,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" t="s">
         <v>23</v>
       </c>
+      <c r="B10"/>
       <c r="C10" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>100</v>
       </c>
       <c r="F10" t="s">
@@ -1124,17 +1105,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>26</v>
       </c>
+      <c r="B11"/>
       <c r="C11" t="s">
         <v>24</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>100</v>
       </c>
       <c r="F11" t="s">
@@ -1159,17 +1141,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" t="s">
         <v>27</v>
       </c>
+      <c r="B12"/>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>100</v>
       </c>
       <c r="F12" t="s">
@@ -1194,17 +1177,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" t="s">
         <v>28</v>
       </c>
+      <c r="B13"/>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13" t="s">
         <v>29</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>100</v>
       </c>
       <c r="F13" t="s">
@@ -1229,17 +1213,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" t="s">
         <v>30</v>
       </c>
+      <c r="B14"/>
       <c r="C14" t="s">
         <v>31</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>100</v>
       </c>
       <c r="F14" t="s">
@@ -1264,17 +1249,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" t="s">
         <v>32</v>
       </c>
+      <c r="B15"/>
       <c r="C15" t="s">
         <v>16</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>100</v>
       </c>
       <c r="F15" t="s">
@@ -1299,17 +1285,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" t="s">
         <v>34</v>
       </c>
+      <c r="B16"/>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>100</v>
       </c>
       <c r="F16" t="s">
@@ -1334,17 +1321,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" t="s">
         <v>36</v>
       </c>
+      <c r="B17"/>
       <c r="C17" t="s">
         <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="n">
         <v>100</v>
       </c>
       <c r="F17" t="s">
@@ -1369,17 +1357,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" t="s">
         <v>37</v>
       </c>
+      <c r="B18"/>
       <c r="C18" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>100</v>
       </c>
       <c r="F18" t="s">
@@ -1404,17 +1393,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" t="s">
         <v>38</v>
       </c>
+      <c r="B19"/>
       <c r="C19" t="s">
         <v>13</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>100</v>
       </c>
       <c r="F19" t="s">
@@ -1439,7 +1429,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1452,7 +1442,7 @@
       <c r="D20" t="s">
         <v>16</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="n">
         <v>100</v>
       </c>
       <c r="F20" t="s">
@@ -1477,17 +1467,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" t="s">
         <v>40</v>
       </c>
+      <c r="B21"/>
       <c r="C21" t="s">
         <v>13</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="n">
         <v>100</v>
       </c>
       <c r="F21" t="s">
@@ -1512,17 +1503,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" t="s">
         <v>41</v>
       </c>
+      <c r="B22"/>
       <c r="C22" t="s">
         <v>13</v>
       </c>
       <c r="D22" t="s">
         <v>35</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="n">
         <v>100</v>
       </c>
       <c r="F22" t="s">
@@ -1547,17 +1539,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" t="s">
         <v>43</v>
       </c>
+      <c r="B23"/>
       <c r="C23" t="s">
         <v>13</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
       </c>
-      <c r="E23">
+      <c r="E23" t="n">
         <v>100</v>
       </c>
       <c r="F23" t="s">
@@ -1582,17 +1575,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" t="s">
         <v>44</v>
       </c>
+      <c r="B24"/>
       <c r="C24" t="s">
         <v>13</v>
       </c>
       <c r="D24" t="s">
         <v>35</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="n">
         <v>100</v>
       </c>
       <c r="F24" t="s">
@@ -1617,17 +1611,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
+      <c r="B25"/>
       <c r="C25" t="s">
         <v>13</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="n">
         <v>100</v>
       </c>
       <c r="F25" t="s">
@@ -1652,17 +1647,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" t="s">
         <v>46</v>
       </c>
+      <c r="B26"/>
       <c r="C26" t="s">
         <v>13</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>100</v>
       </c>
       <c r="F26" t="s">
@@ -1687,17 +1683,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" t="s">
         <v>47</v>
       </c>
+      <c r="B27"/>
       <c r="C27" t="s">
         <v>13</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>100</v>
       </c>
       <c r="F27" t="s">
@@ -1722,7 +1719,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1735,7 +1732,7 @@
       <c r="D28" t="s">
         <v>16</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="n">
         <v>100</v>
       </c>
       <c r="F28" t="s">
@@ -1760,17 +1757,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" t="s">
         <v>49</v>
       </c>
+      <c r="B29"/>
       <c r="C29" t="s">
         <v>13</v>
       </c>
       <c r="D29" t="s">
         <v>14</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="n">
         <v>100</v>
       </c>
       <c r="F29" t="s">
@@ -1795,17 +1793,18 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" t="s">
         <v>50</v>
       </c>
+      <c r="B30"/>
       <c r="C30" t="s">
         <v>13</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="n">
         <v>100</v>
       </c>
       <c r="F30" t="s">
@@ -1830,17 +1829,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" t="s">
         <v>51</v>
       </c>
+      <c r="B31"/>
       <c r="C31" t="s">
         <v>16</v>
       </c>
       <c r="D31" t="s">
         <v>52</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>100</v>
       </c>
       <c r="F31" t="s">
@@ -1865,7 +1865,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -1878,7 +1878,7 @@
       <c r="D32" t="s">
         <v>16</v>
       </c>
-      <c r="E32">
+      <c r="E32" t="n">
         <v>100</v>
       </c>
       <c r="F32" t="s">
@@ -1903,17 +1903,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" t="s">
         <v>54</v>
       </c>
+      <c r="B33"/>
       <c r="C33" t="s">
         <v>13</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
       </c>
-      <c r="E33">
+      <c r="E33" t="n">
         <v>100</v>
       </c>
       <c r="F33" t="s">
@@ -1938,7 +1939,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -1951,7 +1952,7 @@
       <c r="D34" t="s">
         <v>16</v>
       </c>
-      <c r="E34">
+      <c r="E34" t="n">
         <v>100</v>
       </c>
       <c r="F34" t="s">
@@ -1976,17 +1977,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" t="s">
         <v>56</v>
       </c>
+      <c r="B35"/>
       <c r="C35" t="s">
         <v>13</v>
       </c>
       <c r="D35" t="s">
         <v>35</v>
       </c>
-      <c r="E35">
+      <c r="E35" t="n">
         <v>100</v>
       </c>
       <c r="F35" t="s">
@@ -2011,17 +2013,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" t="s">
         <v>57</v>
       </c>
+      <c r="B36"/>
       <c r="C36" t="s">
         <v>13</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
       </c>
-      <c r="E36">
+      <c r="E36" t="n">
         <v>100</v>
       </c>
       <c r="F36" t="s">
@@ -2046,7 +2049,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -2059,7 +2062,7 @@
       <c r="D37" t="s">
         <v>16</v>
       </c>
-      <c r="E37">
+      <c r="E37" t="n">
         <v>100</v>
       </c>
       <c r="F37" t="s">
@@ -2084,17 +2087,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" t="s">
         <v>60</v>
       </c>
+      <c r="B38"/>
       <c r="C38" t="s">
         <v>13</v>
       </c>
       <c r="D38" t="s">
         <v>35</v>
       </c>
-      <c r="E38">
+      <c r="E38" t="n">
         <v>100</v>
       </c>
       <c r="F38" t="s">
@@ -2119,17 +2123,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" t="s">
         <v>61</v>
       </c>
+      <c r="B39"/>
       <c r="C39" t="s">
         <v>13</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
       </c>
-      <c r="E39">
+      <c r="E39" t="n">
         <v>100</v>
       </c>
       <c r="F39" t="s">
@@ -2154,17 +2159,18 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" t="s">
         <v>62</v>
       </c>
+      <c r="B40"/>
       <c r="C40" t="s">
         <v>16</v>
       </c>
       <c r="D40" t="s">
         <v>33</v>
       </c>
-      <c r="E40">
+      <c r="E40" t="n">
         <v>100</v>
       </c>
       <c r="F40" t="s">
@@ -2189,17 +2195,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" t="s">
         <v>63</v>
       </c>
+      <c r="B41"/>
       <c r="C41" t="s">
         <v>16</v>
       </c>
       <c r="D41" t="s">
         <v>33</v>
       </c>
-      <c r="E41">
+      <c r="E41" t="n">
         <v>100</v>
       </c>
       <c r="F41" t="s">
@@ -2224,17 +2231,18 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" t="s">
         <v>64</v>
       </c>
+      <c r="B42"/>
       <c r="C42" t="s">
         <v>13</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
       </c>
-      <c r="E42">
+      <c r="E42" t="n">
         <v>100</v>
       </c>
       <c r="F42" t="s">
@@ -2259,7 +2267,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" t="s">
         <v>65</v>
       </c>
@@ -2272,7 +2280,7 @@
       <c r="D43" t="s">
         <v>16</v>
       </c>
-      <c r="E43">
+      <c r="E43" t="n">
         <v>100</v>
       </c>
       <c r="F43" t="s">
@@ -2297,7 +2305,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -2310,7 +2318,7 @@
       <c r="D44" t="s">
         <v>16</v>
       </c>
-      <c r="E44">
+      <c r="E44" t="n">
         <v>100</v>
       </c>
       <c r="F44" t="s">
@@ -2335,7 +2343,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -2348,7 +2356,7 @@
       <c r="D45" t="s">
         <v>16</v>
       </c>
-      <c r="E45">
+      <c r="E45" t="n">
         <v>100</v>
       </c>
       <c r="F45" t="s">
@@ -2373,7 +2381,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -2386,7 +2394,7 @@
       <c r="D46" t="s">
         <v>16</v>
       </c>
-      <c r="E46">
+      <c r="E46" t="n">
         <v>100</v>
       </c>
       <c r="F46" t="s">
@@ -2411,7 +2419,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -2424,7 +2432,7 @@
       <c r="D47" t="s">
         <v>16</v>
       </c>
-      <c r="E47">
+      <c r="E47" t="n">
         <v>100</v>
       </c>
       <c r="F47" t="s">
@@ -2449,7 +2457,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -2462,7 +2470,7 @@
       <c r="D48" t="s">
         <v>16</v>
       </c>
-      <c r="E48">
+      <c r="E48" t="n">
         <v>100</v>
       </c>
       <c r="F48" t="s">
@@ -2487,17 +2495,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" t="s">
         <v>71</v>
       </c>
+      <c r="B49"/>
       <c r="C49" t="s">
         <v>13</v>
       </c>
       <c r="D49" t="s">
         <v>14</v>
       </c>
-      <c r="E49">
+      <c r="E49" t="n">
         <v>100</v>
       </c>
       <c r="F49" t="s">
@@ -2522,17 +2531,18 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" t="s">
         <v>72</v>
       </c>
+      <c r="B50"/>
       <c r="C50" t="s">
         <v>16</v>
       </c>
       <c r="D50" t="s">
         <v>73</v>
       </c>
-      <c r="E50">
+      <c r="E50" t="n">
         <v>100</v>
       </c>
       <c r="F50" t="s">
@@ -2557,7 +2567,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -2570,7 +2580,7 @@
       <c r="D51" t="s">
         <v>16</v>
       </c>
-      <c r="E51">
+      <c r="E51" t="n">
         <v>100</v>
       </c>
       <c r="F51" t="s">
@@ -2595,17 +2605,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" t="s">
         <v>75</v>
       </c>
+      <c r="B52"/>
       <c r="C52" t="s">
         <v>76</v>
       </c>
       <c r="D52" t="s">
         <v>35</v>
       </c>
-      <c r="E52">
+      <c r="E52" t="n">
         <v>100</v>
       </c>
       <c r="F52" t="s">
@@ -2630,7 +2641,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -2643,7 +2654,7 @@
       <c r="D53" t="s">
         <v>16</v>
       </c>
-      <c r="E53">
+      <c r="E53" t="n">
         <v>100</v>
       </c>
       <c r="F53" t="s">
@@ -2668,17 +2679,18 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" t="s">
         <v>79</v>
       </c>
+      <c r="B54"/>
       <c r="C54" t="s">
         <v>13</v>
       </c>
       <c r="D54" t="s">
         <v>14</v>
       </c>
-      <c r="E54">
+      <c r="E54" t="n">
         <v>100</v>
       </c>
       <c r="F54" t="s">
@@ -2703,17 +2715,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="A55" t="s">
         <v>80</v>
       </c>
+      <c r="B55"/>
       <c r="C55" t="s">
         <v>13</v>
       </c>
       <c r="D55" t="s">
         <v>14</v>
       </c>
-      <c r="E55">
+      <c r="E55" t="n">
         <v>100</v>
       </c>
       <c r="F55" t="s">
@@ -2738,17 +2751,18 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56">
       <c r="A56" t="s">
         <v>81</v>
       </c>
+      <c r="B56"/>
       <c r="C56" t="s">
         <v>13</v>
       </c>
       <c r="D56" t="s">
         <v>14</v>
       </c>
-      <c r="E56">
+      <c r="E56" t="n">
         <v>100</v>
       </c>
       <c r="F56" t="s">
@@ -2773,17 +2787,18 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57">
       <c r="A57" t="s">
         <v>82</v>
       </c>
+      <c r="B57"/>
       <c r="C57" t="s">
         <v>13</v>
       </c>
       <c r="D57" t="s">
         <v>35</v>
       </c>
-      <c r="E57">
+      <c r="E57" t="n">
         <v>100</v>
       </c>
       <c r="F57" t="s">
@@ -2808,17 +2823,18 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58">
       <c r="A58" t="s">
         <v>83</v>
       </c>
+      <c r="B58"/>
       <c r="C58" t="s">
         <v>13</v>
       </c>
       <c r="D58" t="s">
         <v>14</v>
       </c>
-      <c r="E58">
+      <c r="E58" t="n">
         <v>100</v>
       </c>
       <c r="F58" t="s">
@@ -2843,7 +2859,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -2856,7 +2872,7 @@
       <c r="D59" t="s">
         <v>16</v>
       </c>
-      <c r="E59">
+      <c r="E59" t="n">
         <v>100</v>
       </c>
       <c r="F59" t="s">
@@ -2881,17 +2897,18 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60">
       <c r="A60" t="s">
         <v>85</v>
       </c>
+      <c r="B60"/>
       <c r="C60" t="s">
         <v>13</v>
       </c>
       <c r="D60" t="s">
         <v>29</v>
       </c>
-      <c r="E60">
+      <c r="E60" t="n">
         <v>100</v>
       </c>
       <c r="F60" t="s">
@@ -2916,7 +2933,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -2929,7 +2946,7 @@
       <c r="D61" t="s">
         <v>16</v>
       </c>
-      <c r="E61">
+      <c r="E61" t="n">
         <v>100</v>
       </c>
       <c r="F61" t="s">
@@ -2954,7 +2971,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62">
       <c r="A62" t="s">
         <v>87</v>
       </c>
@@ -2967,7 +2984,7 @@
       <c r="D62" t="s">
         <v>16</v>
       </c>
-      <c r="E62">
+      <c r="E62" t="n">
         <v>100</v>
       </c>
       <c r="F62" t="s">
@@ -2992,17 +3009,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63">
       <c r="A63" t="s">
         <v>88</v>
       </c>
+      <c r="B63"/>
       <c r="C63" t="s">
         <v>13</v>
       </c>
       <c r="D63" t="s">
         <v>14</v>
       </c>
-      <c r="E63">
+      <c r="E63" t="n">
         <v>100</v>
       </c>
       <c r="F63" t="s">
@@ -3027,17 +3045,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64">
       <c r="A64" t="s">
         <v>89</v>
       </c>
+      <c r="B64"/>
       <c r="C64" t="s">
         <v>13</v>
       </c>
       <c r="D64" t="s">
         <v>14</v>
       </c>
-      <c r="E64">
+      <c r="E64" t="n">
         <v>100</v>
       </c>
       <c r="F64" t="s">
@@ -3062,17 +3081,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65">
       <c r="A65" t="s">
         <v>90</v>
       </c>
+      <c r="B65"/>
       <c r="C65" t="s">
         <v>13</v>
       </c>
       <c r="D65" t="s">
         <v>14</v>
       </c>
-      <c r="E65">
+      <c r="E65" t="n">
         <v>100</v>
       </c>
       <c r="F65" t="s">
@@ -3097,17 +3117,18 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66">
       <c r="A66" t="s">
         <v>91</v>
       </c>
+      <c r="B66"/>
       <c r="C66" t="s">
         <v>13</v>
       </c>
       <c r="D66" t="s">
         <v>35</v>
       </c>
-      <c r="E66">
+      <c r="E66" t="n">
         <v>100</v>
       </c>
       <c r="F66" t="s">
@@ -3132,17 +3153,18 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67">
       <c r="A67" t="s">
         <v>92</v>
       </c>
+      <c r="B67"/>
       <c r="C67" t="s">
         <v>13</v>
       </c>
       <c r="D67" t="s">
         <v>35</v>
       </c>
-      <c r="E67">
+      <c r="E67" t="n">
         <v>100</v>
       </c>
       <c r="F67" t="s">
@@ -3167,18 +3189,19 @@
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68">
       <c r="A68" t="s">
         <v>93</v>
       </c>
+      <c r="B68"/>
       <c r="C68" t="s">
         <v>13</v>
       </c>
       <c r="D68" t="s">
         <v>14</v>
       </c>
-      <c r="E68">
-        <v>85.714285714285694</v>
+      <c r="E68" t="n">
+        <v>85.7142857142857</v>
       </c>
       <c r="F68" t="s">
         <v>93</v>
@@ -3195,23 +3218,26 @@
       <c r="J68" t="s">
         <v>93</v>
       </c>
+      <c r="K68"/>
       <c r="L68" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69">
       <c r="A69" t="s">
         <v>94</v>
       </c>
+      <c r="B69"/>
       <c r="C69" t="s">
         <v>16</v>
       </c>
       <c r="D69" t="s">
         <v>33</v>
       </c>
-      <c r="E69">
-        <v>85.714285714285694</v>
-      </c>
+      <c r="E69" t="n">
+        <v>85.7142857142857</v>
+      </c>
+      <c r="F69"/>
       <c r="G69" t="s">
         <v>94</v>
       </c>
@@ -3231,18 +3257,19 @@
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70">
       <c r="A70" t="s">
         <v>95</v>
       </c>
+      <c r="B70"/>
       <c r="C70" t="s">
         <v>13</v>
       </c>
       <c r="D70" t="s">
         <v>14</v>
       </c>
-      <c r="E70">
-        <v>85.714285714285694</v>
+      <c r="E70" t="n">
+        <v>85.7142857142857</v>
       </c>
       <c r="F70" t="s">
         <v>95</v>
@@ -3256,6 +3283,7 @@
       <c r="I70" t="s">
         <v>95</v>
       </c>
+      <c r="J70"/>
       <c r="K70" t="s">
         <v>95</v>
       </c>
@@ -3263,7 +3291,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71">
       <c r="A71" t="s">
         <v>96</v>
       </c>
@@ -3276,8 +3304,8 @@
       <c r="D71" t="s">
         <v>16</v>
       </c>
-      <c r="E71">
-        <v>85.714285714285694</v>
+      <c r="E71" t="n">
+        <v>85.7142857142857</v>
       </c>
       <c r="F71" t="s">
         <v>96</v>
@@ -3297,8 +3325,9 @@
       <c r="K71" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L71"/>
+    </row>
+    <row r="72">
       <c r="A72" t="s">
         <v>97</v>
       </c>
@@ -3311,8 +3340,8 @@
       <c r="D72" t="s">
         <v>16</v>
       </c>
-      <c r="E72">
-        <v>85.714285714285694</v>
+      <c r="E72" t="n">
+        <v>85.7142857142857</v>
       </c>
       <c r="F72" t="s">
         <v>97</v>
@@ -3332,8 +3361,9 @@
       <c r="K72" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L72"/>
+    </row>
+    <row r="73">
       <c r="A73" t="s">
         <v>98</v>
       </c>
@@ -3346,8 +3376,8 @@
       <c r="D73" t="s">
         <v>13</v>
       </c>
-      <c r="E73">
-        <v>85.714285714285694</v>
+      <c r="E73" t="n">
+        <v>85.7142857142857</v>
       </c>
       <c r="F73" t="s">
         <v>99</v>
@@ -3367,8 +3397,9 @@
       <c r="K73" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L73"/>
+    </row>
+    <row r="74">
       <c r="A74" t="s">
         <v>100</v>
       </c>
@@ -3381,9 +3412,10 @@
       <c r="D74" t="s">
         <v>16</v>
       </c>
-      <c r="E74">
-        <v>85.714285714285694</v>
-      </c>
+      <c r="E74" t="n">
+        <v>85.7142857142857</v>
+      </c>
+      <c r="F74"/>
       <c r="G74" t="s">
         <v>100</v>
       </c>
@@ -3403,7 +3435,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75">
       <c r="A75" t="s">
         <v>101</v>
       </c>
@@ -3416,9 +3448,10 @@
       <c r="D75" t="s">
         <v>16</v>
       </c>
-      <c r="E75">
-        <v>85.714285714285694</v>
-      </c>
+      <c r="E75" t="n">
+        <v>85.7142857142857</v>
+      </c>
+      <c r="F75"/>
       <c r="G75" t="s">
         <v>101</v>
       </c>
@@ -3438,19 +3471,23 @@
         <v>101</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76">
       <c r="A76" t="s">
         <v>102</v>
       </c>
+      <c r="B76"/>
       <c r="C76" t="s">
         <v>16</v>
       </c>
       <c r="D76" t="s">
         <v>33</v>
       </c>
-      <c r="E76">
-        <v>57.142857142857103</v>
-      </c>
+      <c r="E76" t="n">
+        <v>57.1428571428571</v>
+      </c>
+      <c r="F76"/>
+      <c r="G76"/>
+      <c r="H76"/>
       <c r="I76" t="s">
         <v>102</v>
       </c>
@@ -3464,22 +3501,27 @@
         <v>102</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77">
       <c r="A77" t="s">
         <v>103</v>
       </c>
+      <c r="B77"/>
       <c r="C77" t="s">
         <v>35</v>
       </c>
       <c r="D77" t="s">
         <v>35</v>
       </c>
-      <c r="E77">
-        <v>42.857142857142897</v>
-      </c>
+      <c r="E77" t="n">
+        <v>42.8571428571429</v>
+      </c>
+      <c r="F77"/>
+      <c r="G77"/>
+      <c r="H77"/>
       <c r="I77" t="s">
         <v>103</v>
       </c>
+      <c r="J77"/>
       <c r="K77" t="s">
         <v>103</v>
       </c>
@@ -3487,7 +3529,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78">
       <c r="A78" t="s">
         <v>104</v>
       </c>
@@ -3500,14 +3542,20 @@
       <c r="D78" t="s">
         <v>105</v>
       </c>
-      <c r="E78">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E78" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F78"/>
+      <c r="G78"/>
+      <c r="H78"/>
+      <c r="I78"/>
+      <c r="J78"/>
+      <c r="K78"/>
       <c r="L78" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79">
       <c r="A79" t="s">
         <v>106</v>
       </c>
@@ -3520,14 +3568,20 @@
       <c r="D79" t="s">
         <v>13</v>
       </c>
-      <c r="E79">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E79" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F79"/>
+      <c r="G79"/>
+      <c r="H79"/>
+      <c r="I79"/>
+      <c r="J79"/>
       <c r="K79" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L79"/>
+    </row>
+    <row r="80">
       <c r="A80" t="s">
         <v>107</v>
       </c>
@@ -3540,14 +3594,20 @@
       <c r="D80" t="s">
         <v>108</v>
       </c>
-      <c r="E80">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E80" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F80"/>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80"/>
+      <c r="J80"/>
+      <c r="K80"/>
       <c r="L80" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81">
       <c r="A81" t="s">
         <v>110</v>
       </c>
@@ -3560,14 +3620,20 @@
       <c r="D81" t="s">
         <v>13</v>
       </c>
-      <c r="E81">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E81" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F81"/>
+      <c r="G81"/>
+      <c r="H81"/>
+      <c r="I81"/>
       <c r="J81" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K81"/>
+      <c r="L81"/>
+    </row>
+    <row r="82">
       <c r="A82" t="s">
         <v>111</v>
       </c>
@@ -3580,14 +3646,20 @@
       <c r="D82" t="s">
         <v>108</v>
       </c>
-      <c r="E82">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E82" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F82"/>
+      <c r="G82"/>
+      <c r="H82"/>
+      <c r="I82"/>
+      <c r="J82"/>
+      <c r="K82"/>
       <c r="L82" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83">
       <c r="A83" t="s">
         <v>112</v>
       </c>
@@ -3600,14 +3672,20 @@
       <c r="D83" t="s">
         <v>105</v>
       </c>
-      <c r="E83">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E83" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F83"/>
+      <c r="G83"/>
+      <c r="H83"/>
+      <c r="I83"/>
+      <c r="J83"/>
+      <c r="K83"/>
       <c r="L83" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84">
       <c r="A84" t="s">
         <v>113</v>
       </c>
@@ -3620,14 +3698,20 @@
       <c r="D84" t="s">
         <v>105</v>
       </c>
-      <c r="E84">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E84" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F84"/>
+      <c r="G84"/>
+      <c r="H84"/>
+      <c r="I84"/>
+      <c r="J84"/>
+      <c r="K84"/>
       <c r="L84" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85">
       <c r="A85" t="s">
         <v>114</v>
       </c>
@@ -3640,14 +3724,20 @@
       <c r="D85" t="s">
         <v>105</v>
       </c>
-      <c r="E85">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E85" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F85"/>
+      <c r="G85"/>
+      <c r="H85"/>
+      <c r="I85"/>
+      <c r="J85"/>
+      <c r="K85"/>
       <c r="L85" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86">
       <c r="A86" t="s">
         <v>116</v>
       </c>
@@ -3660,14 +3750,20 @@
       <c r="D86" t="s">
         <v>105</v>
       </c>
-      <c r="E86">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E86" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86"/>
+      <c r="J86"/>
+      <c r="K86"/>
       <c r="L86" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87">
       <c r="A87" t="s">
         <v>118</v>
       </c>
@@ -3680,14 +3776,20 @@
       <c r="D87" t="s">
         <v>105</v>
       </c>
-      <c r="E87">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E87" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F87"/>
+      <c r="G87"/>
+      <c r="H87"/>
+      <c r="I87"/>
+      <c r="J87"/>
+      <c r="K87"/>
       <c r="L87" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88">
       <c r="A88" t="s">
         <v>119</v>
       </c>
@@ -3700,14 +3802,20 @@
       <c r="D88" t="s">
         <v>105</v>
       </c>
-      <c r="E88">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E88" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="I88"/>
+      <c r="J88"/>
+      <c r="K88"/>
       <c r="L88" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89">
       <c r="A89" t="s">
         <v>120</v>
       </c>
@@ -3720,14 +3828,20 @@
       <c r="D89" t="s">
         <v>108</v>
       </c>
-      <c r="E89">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E89" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
+      <c r="J89"/>
+      <c r="K89"/>
       <c r="L89" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90">
       <c r="A90" t="s">
         <v>122</v>
       </c>
@@ -3740,14 +3854,20 @@
       <c r="D90" t="s">
         <v>16</v>
       </c>
-      <c r="E90">
-        <v>14.285714285714301</v>
+      <c r="E90" t="n">
+        <v>14.2857142857143</v>
       </c>
       <c r="F90" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+      <c r="J90"/>
+      <c r="K90"/>
+      <c r="L90"/>
+    </row>
+    <row r="91">
       <c r="A91" t="s">
         <v>123</v>
       </c>
@@ -3760,14 +3880,20 @@
       <c r="D91" t="s">
         <v>108</v>
       </c>
-      <c r="E91">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E91" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F91"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="I91"/>
+      <c r="J91"/>
+      <c r="K91"/>
       <c r="L91" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92">
       <c r="A92" t="s">
         <v>124</v>
       </c>
@@ -3780,14 +3906,20 @@
       <c r="D92" t="s">
         <v>16</v>
       </c>
-      <c r="E92">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E92" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F92"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="I92"/>
+      <c r="J92"/>
+      <c r="K92"/>
       <c r="L92" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93">
       <c r="A93" t="s">
         <v>125</v>
       </c>
@@ -3800,14 +3932,20 @@
       <c r="D93" t="s">
         <v>105</v>
       </c>
-      <c r="E93">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E93" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93"/>
+      <c r="J93"/>
+      <c r="K93"/>
       <c r="L93" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94">
       <c r="A94" t="s">
         <v>126</v>
       </c>
@@ -3820,14 +3958,20 @@
       <c r="D94" t="s">
         <v>108</v>
       </c>
-      <c r="E94">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E94" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94"/>
+      <c r="K94"/>
       <c r="L94" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95">
       <c r="A95" t="s">
         <v>127</v>
       </c>
@@ -3840,28 +3984,34 @@
       <c r="D95" t="s">
         <v>108</v>
       </c>
-      <c r="E95">
-        <v>14.285714285714301</v>
-      </c>
+      <c r="E95" t="n">
+        <v>14.2857142857143</v>
+      </c>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+      <c r="J95"/>
+      <c r="K95"/>
       <c r="L95" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H95"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3887,7 +4037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3913,7 +4063,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -3939,7 +4089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3965,7 +4115,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3991,7 +4141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -4017,7 +4167,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -4043,7 +4193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -4069,7 +4219,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -4095,7 +4245,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -4121,7 +4271,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -4147,7 +4297,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -4173,7 +4323,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -4199,7 +4349,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -4225,7 +4375,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -4251,7 +4401,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -4277,7 +4427,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -4303,7 +4453,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -4329,7 +4479,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -4355,7 +4505,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -4381,7 +4531,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -4407,7 +4557,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -4433,7 +4583,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -4459,7 +4609,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -4485,7 +4635,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -4511,7 +4661,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -4537,7 +4687,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -4563,7 +4713,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -4589,7 +4739,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -4615,7 +4765,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -4641,7 +4791,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -4667,7 +4817,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -4693,7 +4843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -4719,7 +4869,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -4745,7 +4895,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -4771,7 +4921,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -4797,7 +4947,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -4823,7 +4973,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" t="s">
         <v>60</v>
       </c>
@@ -4849,7 +4999,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" t="s">
         <v>61</v>
       </c>
@@ -4875,7 +5025,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -4901,7 +5051,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -4927,7 +5077,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -4953,7 +5103,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" t="s">
         <v>65</v>
       </c>
@@ -4979,7 +5129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -5005,7 +5155,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -5031,7 +5181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -5057,7 +5207,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -5083,7 +5233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -5109,7 +5259,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" t="s">
         <v>71</v>
       </c>
@@ -5135,7 +5285,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -5161,7 +5311,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -5187,7 +5337,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" t="s">
         <v>75</v>
       </c>
@@ -5213,7 +5363,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -5239,7 +5389,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" t="s">
         <v>79</v>
       </c>
@@ -5265,7 +5415,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="A55" t="s">
         <v>80</v>
       </c>
@@ -5291,7 +5441,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56">
       <c r="A56" t="s">
         <v>81</v>
       </c>
@@ -5317,7 +5467,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -5343,7 +5493,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58">
       <c r="A58" t="s">
         <v>83</v>
       </c>
@@ -5369,7 +5519,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -5395,7 +5545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60">
       <c r="A60" t="s">
         <v>85</v>
       </c>
@@ -5421,7 +5571,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -5447,7 +5597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62">
       <c r="A62" t="s">
         <v>87</v>
       </c>
@@ -5473,7 +5623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -5499,7 +5649,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -5525,7 +5675,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65">
       <c r="A65" t="s">
         <v>90</v>
       </c>
@@ -5551,7 +5701,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66">
       <c r="A66" t="s">
         <v>91</v>
       </c>
@@ -5577,7 +5727,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67">
       <c r="A67" t="s">
         <v>92</v>
       </c>
@@ -5603,7 +5753,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68">
       <c r="A68" t="s">
         <v>93</v>
       </c>
@@ -5622,14 +5772,16 @@
       <c r="F68" t="s">
         <v>13</v>
       </c>
+      <c r="G68"/>
       <c r="H68" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69">
       <c r="A69" t="s">
         <v>94</v>
       </c>
+      <c r="B69"/>
       <c r="C69" t="s">
         <v>16</v>
       </c>
@@ -5649,7 +5801,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70">
       <c r="A70" t="s">
         <v>95</v>
       </c>
@@ -5665,6 +5817,7 @@
       <c r="E70" t="s">
         <v>13</v>
       </c>
+      <c r="F70"/>
       <c r="G70" t="s">
         <v>13</v>
       </c>
@@ -5672,7 +5825,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71">
       <c r="A71" t="s">
         <v>96</v>
       </c>
@@ -5694,8 +5847,9 @@
       <c r="G71" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H71"/>
+    </row>
+    <row r="72">
       <c r="A72" t="s">
         <v>97</v>
       </c>
@@ -5717,8 +5871,9 @@
       <c r="G72" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H72"/>
+    </row>
+    <row r="73">
       <c r="A73" t="s">
         <v>98</v>
       </c>
@@ -5740,11 +5895,13 @@
       <c r="G73" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H73"/>
+    </row>
+    <row r="74">
       <c r="A74" t="s">
         <v>100</v>
       </c>
+      <c r="B74"/>
       <c r="C74" t="s">
         <v>16</v>
       </c>
@@ -5764,10 +5921,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75">
       <c r="A75" t="s">
         <v>101</v>
       </c>
+      <c r="B75"/>
       <c r="C75" t="s">
         <v>16</v>
       </c>
@@ -5787,10 +5945,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76">
       <c r="A76" t="s">
         <v>102</v>
       </c>
+      <c r="B76"/>
+      <c r="C76"/>
+      <c r="D76"/>
       <c r="E76" t="s">
         <v>16</v>
       </c>
@@ -5804,13 +5965,17 @@
         <v>105</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77">
       <c r="A77" t="s">
         <v>103</v>
       </c>
+      <c r="B77"/>
+      <c r="C77"/>
+      <c r="D77"/>
       <c r="E77" t="s">
         <v>13</v>
       </c>
+      <c r="F77"/>
       <c r="G77" t="s">
         <v>16</v>
       </c>
@@ -5818,152 +5983,260 @@
         <v>105</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78">
       <c r="A78" t="s">
         <v>104</v>
       </c>
+      <c r="B78"/>
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
       <c r="H78" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79">
       <c r="A79" t="s">
         <v>106</v>
       </c>
+      <c r="B79"/>
+      <c r="C79"/>
+      <c r="D79"/>
+      <c r="E79"/>
+      <c r="F79"/>
       <c r="G79" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H79"/>
+    </row>
+    <row r="80">
       <c r="A80" t="s">
         <v>107</v>
       </c>
+      <c r="B80"/>
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
       <c r="H80" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81">
       <c r="A81" t="s">
         <v>110</v>
       </c>
+      <c r="B81"/>
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="E81"/>
       <c r="F81" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G81"/>
+      <c r="H81"/>
+    </row>
+    <row r="82">
       <c r="A82" t="s">
         <v>111</v>
       </c>
+      <c r="B82"/>
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="G82"/>
       <c r="H82" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83">
       <c r="A83" t="s">
         <v>112</v>
       </c>
+      <c r="B83"/>
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
       <c r="H83" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84">
       <c r="A84" t="s">
         <v>113</v>
       </c>
+      <c r="B84"/>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
       <c r="H84" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85">
       <c r="A85" t="s">
         <v>114</v>
       </c>
+      <c r="B85"/>
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
       <c r="H85" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86">
       <c r="A86" t="s">
         <v>116</v>
       </c>
+      <c r="B86"/>
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
       <c r="H86" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87">
       <c r="A87" t="s">
         <v>118</v>
       </c>
+      <c r="B87"/>
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="E87"/>
+      <c r="F87"/>
+      <c r="G87"/>
       <c r="H87" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88">
       <c r="A88" t="s">
         <v>119</v>
       </c>
+      <c r="B88"/>
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
       <c r="H88" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89">
       <c r="A89" t="s">
         <v>120</v>
       </c>
+      <c r="B89"/>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
       <c r="H89" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90">
       <c r="A90" t="s">
         <v>122</v>
       </c>
       <c r="B90" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+    </row>
+    <row r="91">
       <c r="A91" t="s">
         <v>123</v>
       </c>
+      <c r="B91"/>
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
       <c r="H91" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92">
       <c r="A92" t="s">
         <v>124</v>
       </c>
+      <c r="B92"/>
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="G92"/>
       <c r="H92" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93">
       <c r="A93" t="s">
         <v>125</v>
       </c>
+      <c r="B93"/>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93"/>
       <c r="H93" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94">
       <c r="A94" t="s">
         <v>126</v>
       </c>
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94"/>
+      <c r="G94"/>
       <c r="H94" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95">
       <c r="A95" t="s">
         <v>127</v>
       </c>
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
       <c r="H95" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>